<commit_message>
Equipment section - content adding
</commit_message>
<xml_diff>
--- a/assets/docs/06 - Institution_METRO's Culture in Transit Productivity Statistics.xlsx
+++ b/assets/docs/06 - Institution_METRO's Culture in Transit Productivity Statistics.xlsx
@@ -943,7 +943,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1669,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>45</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>48</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>50</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>53</v>
       </c>
@@ -1847,7 +1847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2327,7 +2329,7 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>45</v>
       </c>
@@ -2340,7 +2342,7 @@
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>48</v>
       </c>
@@ -2352,7 +2354,7 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>130</v>
       </c>
@@ -2360,7 +2362,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="69" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>53</v>
       </c>
@@ -2409,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2723,7 +2725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>45</v>
       </c>
@@ -2731,7 +2733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
@@ -2739,7 +2741,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>50</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>53</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>59</v>
       </c>
@@ -2796,7 +2798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3125,7 +3129,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>45</v>
       </c>
@@ -3133,7 +3137,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>48</v>
       </c>
@@ -3141,7 +3145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>50</v>
       </c>
@@ -3149,7 +3153,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>53</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>61</v>
       </c>
@@ -3176,7 +3180,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>63</v>
       </c>
@@ -3198,7 +3202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3533,7 +3539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>45</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>48</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>50</v>
       </c>
@@ -3557,7 +3563,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>53</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>59</v>
       </c>
@@ -3576,7 +3582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>61</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>63</v>
       </c>
@@ -3606,7 +3612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3827,7 +3835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>45</v>
       </c>
@@ -3835,7 +3843,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>48</v>
       </c>
@@ -3843,7 +3851,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>50</v>
       </c>
@@ -3851,7 +3859,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>53</v>
       </c>
@@ -3870,7 +3878,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>61</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>63</v>
       </c>
@@ -3900,7 +3908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4209,7 +4219,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>45</v>
       </c>
@@ -4220,7 +4230,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>48</v>
       </c>
@@ -4231,7 +4241,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>50</v>
       </c>
@@ -4242,7 +4252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>53</v>
       </c>
@@ -4264,7 +4274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>61</v>
       </c>
@@ -4272,7 +4282,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>63</v>
       </c>
@@ -4294,7 +4304,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4540,7 +4552,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>45</v>
       </c>
@@ -4551,7 +4563,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>48</v>
       </c>
@@ -4562,7 +4574,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>50</v>
       </c>
@@ -4573,7 +4585,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>53</v>
       </c>
@@ -4585,7 +4597,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>59</v>
       </c>
@@ -4593,7 +4605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>61</v>
       </c>
@@ -4601,7 +4613,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>63</v>
       </c>
@@ -4624,7 +4636,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5015,7 +5027,7 @@
       <c r="H19" s="22"/>
       <c r="J19" s="22"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>45</v>
       </c>
@@ -5025,7 +5037,7 @@
       <c r="C20" s="40"/>
       <c r="D20" s="22"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>48</v>
       </c>
@@ -5034,7 +5046,7 @@
       </c>
       <c r="C21" s="40"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>50</v>
       </c>
@@ -5043,7 +5055,7 @@
       </c>
       <c r="C22" s="40"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>53</v>
       </c>
@@ -5063,7 +5075,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>61</v>
       </c>
@@ -5071,7 +5083,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>63</v>
       </c>
@@ -5093,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change to file in institution section
</commit_message>
<xml_diff>
--- a/assets/docs/06 - Institution_METRO's Culture in Transit Productivity Statistics.xlsx
+++ b/assets/docs/06 - Institution_METRO's Culture in Transit Productivity Statistics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="480" windowWidth="22716" windowHeight="11052" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="132" yWindow="480" windowWidth="22716" windowHeight="11052" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WCS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="145">
   <si>
     <t>White Plains Public Library</t>
   </si>
@@ -31,9 +31,6 @@
     <t>The New York Academy of Medicine Library</t>
   </si>
   <si>
-    <t>Wildlife Conservation Society Archives</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -443,6 +440,24 @@
   </si>
   <si>
     <t>General Society of Mechanics and Tradesmen</t>
+  </si>
+  <si>
+    <t>(119 items were digitized but after review during post-processing work 7 items were deemed unusable for online display)</t>
+  </si>
+  <si>
+    <t>Wildlife Conservation Society Archives - Culture in Transit Pilot Institution</t>
+  </si>
+  <si>
+    <t>(402 digital images were produced but after review during post-processing work 12 image files were deemed unusable for online display)</t>
+  </si>
+  <si>
+    <t>White Plains community scanning day</t>
+  </si>
+  <si>
+    <t>76 additional items were digitized during a community scanning day, so the total amount of items in the DCMNY White Plains collection is 322.</t>
+  </si>
+  <si>
+    <t>This includes 101 images that were digitized as part of the White Plains community scanning day.</t>
   </si>
 </sst>
 </file>
@@ -551,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -639,6 +654,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,7 +962,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -963,7 +982,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="7"/>
@@ -989,38 +1008,38 @@
     </row>
     <row r="3" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1054,7 +1073,7 @@
       </c>
       <c r="K4" s="14"/>
       <c r="M4" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1088,7 +1107,7 @@
       </c>
       <c r="K5" s="14"/>
       <c r="M5" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1122,7 +1141,7 @@
       </c>
       <c r="K6" s="14"/>
       <c r="M6" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,7 +1175,7 @@
       </c>
       <c r="K7" s="14"/>
       <c r="M7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,10 +1208,10 @@
         <v>12</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1226,7 +1245,7 @@
       </c>
       <c r="K9" s="14"/>
       <c r="M9" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1259,10 +1278,10 @@
         <v>2</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1296,7 +1315,7 @@
       </c>
       <c r="K11" s="14"/>
       <c r="M11" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1330,7 +1349,7 @@
       </c>
       <c r="K12" s="14"/>
       <c r="M12" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1363,10 +1382,10 @@
         <v>1</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1374,13 +1393,13 @@
         <v>42193</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="16">
@@ -1390,19 +1409,19 @@
         <v>0</v>
       </c>
       <c r="H14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,35 +1429,35 @@
         <v>42194</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="16">
         <v>115</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1446,35 +1465,35 @@
         <v>42195</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="16">
         <v>275</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1482,35 +1501,35 @@
         <v>42198</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1518,40 +1537,40 @@
         <v>42199</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="20">
         <f t="shared" ref="B19:D19" si="0">SUM(B4:B18)</f>
@@ -1587,7 +1606,7 @@
       </c>
       <c r="K19" s="14"/>
       <c r="M19" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1599,23 +1618,25 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="M20" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="29">
-        <v>119</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>112</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="H21" s="7"/>
@@ -1625,13 +1646,15 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="29">
-        <v>402</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>390</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="H22" s="7"/>
@@ -1653,10 +1676,10 @@
     </row>
     <row r="24" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1666,15 +1689,15 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="M24" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1685,15 +1708,15 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="M25" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1704,12 +1727,12 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1720,16 +1743,16 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1740,10 +1763,10 @@
     </row>
     <row r="29" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1756,10 +1779,10 @@
     </row>
     <row r="30" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="7"/>
@@ -1772,10 +1795,10 @@
     </row>
     <row r="31" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>64</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="7"/>
@@ -1833,7 +1856,7 @@
       <c r="B37" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection password="9E2D" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A22:B22"/>
@@ -1847,9 +1870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1869,43 +1890,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,10 +1951,10 @@
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1964,10 +1985,10 @@
         <v>2</v>
       </c>
       <c r="K5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1996,10 +2017,10 @@
         <v>16</v>
       </c>
       <c r="K6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2026,7 +2047,7 @@
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M7" s="13"/>
     </row>
@@ -2052,7 +2073,7 @@
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M8" s="13"/>
     </row>
@@ -2115,7 +2136,7 @@
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="13">
         <v>115</v>
@@ -2134,7 +2155,7 @@
         <v>6</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M11" s="13"/>
     </row>
@@ -2189,7 +2210,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2208,7 +2229,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2227,7 +2248,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2246,7 +2267,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2265,7 +2286,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2299,7 +2320,7 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="22">
@@ -2308,7 +2329,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="22">
@@ -2317,10 +2338,10 @@
     </row>
     <row r="24" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="22"/>
       <c r="G24" s="22"/>
@@ -2329,12 +2350,12 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
     </row>
-    <row r="25" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="22"/>
       <c r="G25" s="22"/>
@@ -2342,59 +2363,59 @@
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
     </row>
-    <row r="26" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
     </row>
-    <row r="27" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="69" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2411,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2435,29 +2456,29 @@
     </row>
     <row r="3" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="J3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2478,7 +2499,7 @@
       </c>
       <c r="H4" s="14"/>
       <c r="J4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2563,7 @@
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,7 +2579,7 @@
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,7 +2595,7 @@
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2590,7 +2611,7 @@
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2606,7 +2627,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2622,7 +2643,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,7 +2657,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,7 +2671,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2664,7 +2685,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2679,7 +2700,7 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="19">
         <v>446</v>
@@ -2701,7 +2722,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="22">
@@ -2710,7 +2731,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="22">
@@ -2719,69 +2740,69 @@
     </row>
     <row r="23" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="B24" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="25" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="B26" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2796,10 +2817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2822,32 +2843,32 @@
     </row>
     <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2868,10 +2889,10 @@
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2893,7 +2914,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="13"/>
       <c r="K5" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,7 +3013,7 @@
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3007,7 +3028,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3028,7 +3049,7 @@
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3045,7 +3066,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3062,7 +3083,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3077,12 +3098,12 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="19">
         <v>242</v>
@@ -3103,96 +3124,125 @@
       <c r="H16" s="20"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="22">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="22">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="24" t="s">
+    <row r="17" spans="1:9" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+    </row>
+    <row r="18" spans="1:9" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="22">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="47"/>
+      <c r="C21" s="22">
+        <v>347</v>
+      </c>
+      <c r="D21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="B24" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="B25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="25" t="s">
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="B26" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="B27" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="16" t="s">
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="B29" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>64</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection password="9E2D" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3202,9 +3252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3222,40 +3270,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="L3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3266,7 +3314,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13">
         <v>32</v>
@@ -3283,10 +3331,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3297,7 +3345,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="13">
         <v>15</v>
@@ -3314,10 +3362,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3328,7 +3376,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="13">
         <v>33</v>
@@ -3346,7 +3394,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3361,10 +3409,10 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3375,7 +3423,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="13">
         <v>59</v>
@@ -3401,7 +3449,7 @@
         <v>78</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="13">
         <v>78</v>
@@ -3428,7 +3476,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3482,18 +3530,18 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="19">
         <v>217</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="19">
         <v>217</v>
@@ -3515,7 +3563,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="22">
@@ -3524,7 +3572,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="22">
@@ -3533,69 +3581,69 @@
     </row>
     <row r="19" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="B20" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>88</v>
-      </c>
       <c r="D23" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="16" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="B25" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3612,9 +3660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3633,40 +3679,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="L3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3687,7 +3733,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="L4" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3735,7 +3781,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3756,7 +3802,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3780,12 +3826,12 @@
         <v>5</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19">
         <v>92</v>
@@ -3811,7 +3857,7 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="22">
@@ -3820,7 +3866,7 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="22">
@@ -3829,69 +3875,69 @@
     </row>
     <row r="14" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="B15" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="41.4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="16" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="B20" s="26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3908,9 +3954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3927,37 +3971,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K3" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3981,7 +4025,7 @@
       </c>
       <c r="I4" s="13"/>
       <c r="K4" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4007,7 +4051,7 @@
       </c>
       <c r="I5" s="13"/>
       <c r="K5" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4165,12 +4209,12 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="19">
         <v>640</v>
@@ -4195,7 +4239,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="22">
@@ -4204,7 +4248,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="22">
@@ -4213,81 +4257,81 @@
     </row>
     <row r="19" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="B20" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="16" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="B25" s="26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4304,9 +4348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4323,37 +4365,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="K3" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4378,10 +4420,10 @@
         <v>20</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4406,7 +4448,7 @@
         <v>33</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4477,7 +4519,7 @@
         <v>45</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4502,7 +4544,7 @@
         <v>13</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4528,7 +4570,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="22">
@@ -4537,7 +4579,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="22">
@@ -4546,79 +4588,79 @@
     </row>
     <row r="15" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="B16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="38"/>
       <c r="F19" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="16" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="B21" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4636,7 +4678,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4656,43 +4698,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="M3" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4721,10 +4763,10 @@
         <v>2</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4754,7 +4796,7 @@
       </c>
       <c r="K5" s="14"/>
       <c r="M5" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4786,7 +4828,7 @@
       </c>
       <c r="K6" s="14"/>
       <c r="M6" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4816,7 +4858,7 @@
       </c>
       <c r="K7" s="13"/>
       <c r="M7" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4874,7 +4916,7 @@
         <v>5</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4903,7 +4945,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4922,7 +4964,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4941,7 +4983,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4960,7 +5002,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4994,7 +5036,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="22">
@@ -5003,7 +5045,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="22">
@@ -5017,78 +5059,78 @@
     </row>
     <row r="19" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="30"/>
       <c r="E19" s="22"/>
       <c r="H19" s="22"/>
       <c r="J19" s="22"/>
     </row>
-    <row r="20" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="22"/>
     </row>
-    <row r="21" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21" s="40"/>
     </row>
-    <row r="22" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="40"/>
     </row>
-    <row r="23" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="40"/>
       <c r="E23" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="16" t="s">
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="B25" s="26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -5105,8 +5147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5125,43 +5167,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5175,7 +5217,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="13">
         <v>74</v>
@@ -5192,10 +5234,10 @@
         <v>15</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5209,7 +5251,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="13">
         <v>147</v>
@@ -5226,10 +5268,10 @@
         <v>17</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5243,7 +5285,7 @@
         <v>44</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="13">
         <v>126</v>
@@ -5260,10 +5302,10 @@
         <v>44</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5277,7 +5319,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="13">
         <v>140</v>
@@ -5294,10 +5336,10 @@
         <v>13</v>
       </c>
       <c r="K7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5305,10 +5347,10 @@
         <v>42489</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="13">
         <v>92</v>
@@ -5331,7 +5373,7 @@
       </c>
       <c r="K8" s="14"/>
       <c r="M8" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5339,33 +5381,33 @@
         <v>42492</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5373,10 +5415,10 @@
         <v>42493</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="13">
         <v>23</v>
@@ -5396,10 +5438,10 @@
         <v>13</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5407,10 +5449,10 @@
         <v>42499</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="13">
         <v>37</v>
@@ -5430,10 +5472,10 @@
         <v>37</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5441,33 +5483,33 @@
         <v>42500</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5504,10 +5546,10 @@
         <v>42502</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="13">
         <v>3</v>
@@ -5529,7 +5571,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5548,7 +5590,7 @@
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
       <c r="K15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5567,7 +5609,7 @@
       <c r="I16" s="41"/>
       <c r="J16" s="41"/>
       <c r="K16" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5586,7 +5628,7 @@
       <c r="I17" s="41"/>
       <c r="J17" s="41"/>
       <c r="K17" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5605,7 +5647,7 @@
       <c r="I18" s="41"/>
       <c r="J18" s="41"/>
       <c r="K18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5624,7 +5666,7 @@
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
       <c r="K19" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5643,7 +5685,7 @@
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
       <c r="K20" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5656,13 +5698,13 @@
       <c r="E21" s="41"/>
       <c r="F21" s="14"/>
       <c r="G21" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="41"/>
       <c r="J21" s="41"/>
       <c r="K21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5679,7 +5721,7 @@
       <c r="I22" s="41"/>
       <c r="J22" s="41"/>
       <c r="K22" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5696,7 +5738,7 @@
       <c r="I23" s="41"/>
       <c r="J23" s="41"/>
       <c r="K23" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5715,7 +5757,7 @@
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H24" s="36">
         <v>364</v>
@@ -5733,7 +5775,7 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="22">
@@ -5746,7 +5788,7 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="47"/>
       <c r="C27" s="22">
@@ -5767,10 +5809,10 @@
     </row>
     <row r="29" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="22"/>
       <c r="H29" s="43"/>
@@ -5779,10 +5821,10 @@
     </row>
     <row r="30" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E30" s="43"/>
       <c r="F30" s="44"/>
@@ -5793,53 +5835,53 @@
     </row>
     <row r="31" spans="1:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>